<commit_message>
Ajout des données du mois d'août
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -444,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W103"/>
+  <dimension ref="A1:W134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3113,6 +3113,848 @@
         <v>29000</v>
       </c>
     </row>
+    <row r="104" spans="1:23">
+      <c r="A104" s="2">
+        <v>45139</v>
+      </c>
+      <c r="D104">
+        <v>6500</v>
+      </c>
+      <c r="F104">
+        <v>5000</v>
+      </c>
+      <c r="I104">
+        <v>10500</v>
+      </c>
+      <c r="J104">
+        <v>1000</v>
+      </c>
+      <c r="R104">
+        <v>1000</v>
+      </c>
+      <c r="S104">
+        <v>18000</v>
+      </c>
+      <c r="V104">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:23">
+      <c r="A105" s="2">
+        <v>45140</v>
+      </c>
+      <c r="B105">
+        <v>100000</v>
+      </c>
+      <c r="C105">
+        <v>5000</v>
+      </c>
+      <c r="D105">
+        <v>204500</v>
+      </c>
+      <c r="F105">
+        <v>272900</v>
+      </c>
+      <c r="K105">
+        <v>110000</v>
+      </c>
+      <c r="R105">
+        <v>9500</v>
+      </c>
+      <c r="S105">
+        <v>1600</v>
+      </c>
+      <c r="U105">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:23">
+      <c r="A106" s="2">
+        <v>45141</v>
+      </c>
+      <c r="C106">
+        <v>92000</v>
+      </c>
+      <c r="D106">
+        <v>177050</v>
+      </c>
+      <c r="E106">
+        <v>39550</v>
+      </c>
+      <c r="F106">
+        <v>23500</v>
+      </c>
+      <c r="I106">
+        <v>5250</v>
+      </c>
+      <c r="J106">
+        <v>1000</v>
+      </c>
+      <c r="K106">
+        <v>50000</v>
+      </c>
+      <c r="O106">
+        <v>5000</v>
+      </c>
+      <c r="R106">
+        <v>4000</v>
+      </c>
+      <c r="S106">
+        <v>9000</v>
+      </c>
+      <c r="T106">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="107" spans="1:23">
+      <c r="A107" s="2">
+        <v>45142</v>
+      </c>
+      <c r="D107">
+        <v>83975</v>
+      </c>
+      <c r="E107">
+        <v>63025</v>
+      </c>
+      <c r="F107">
+        <v>226400</v>
+      </c>
+      <c r="I107">
+        <v>3500</v>
+      </c>
+      <c r="J107">
+        <v>1000</v>
+      </c>
+      <c r="M107">
+        <v>75000</v>
+      </c>
+      <c r="R107">
+        <v>24100</v>
+      </c>
+      <c r="T107">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:23">
+      <c r="A108" s="2">
+        <v>45143</v>
+      </c>
+      <c r="D108">
+        <v>107350</v>
+      </c>
+      <c r="F108">
+        <v>297200</v>
+      </c>
+      <c r="I108">
+        <v>4500</v>
+      </c>
+      <c r="J108">
+        <v>1000</v>
+      </c>
+      <c r="N108">
+        <v>9000</v>
+      </c>
+      <c r="R108">
+        <v>3600</v>
+      </c>
+      <c r="U108">
+        <v>25000</v>
+      </c>
+      <c r="V108">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="109" spans="1:23">
+      <c r="A109" s="2">
+        <v>45144</v>
+      </c>
+      <c r="C109">
+        <v>1000</v>
+      </c>
+      <c r="D109">
+        <v>73750</v>
+      </c>
+      <c r="F109">
+        <v>33400</v>
+      </c>
+      <c r="G109">
+        <v>1890450</v>
+      </c>
+      <c r="I109">
+        <v>3500</v>
+      </c>
+      <c r="J109">
+        <v>1000</v>
+      </c>
+      <c r="R109">
+        <v>9000</v>
+      </c>
+      <c r="S109">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:23">
+      <c r="A110" s="2">
+        <v>45145</v>
+      </c>
+      <c r="C110">
+        <v>92000</v>
+      </c>
+      <c r="D110">
+        <v>191950</v>
+      </c>
+      <c r="I110">
+        <v>2000</v>
+      </c>
+      <c r="J110">
+        <v>1000</v>
+      </c>
+      <c r="Q110">
+        <v>3000</v>
+      </c>
+      <c r="R110">
+        <v>500</v>
+      </c>
+      <c r="U110">
+        <v>20000</v>
+      </c>
+      <c r="V110">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:23">
+      <c r="A111" s="2">
+        <v>45146</v>
+      </c>
+      <c r="C111">
+        <v>1500</v>
+      </c>
+      <c r="D111">
+        <v>64000</v>
+      </c>
+      <c r="F111">
+        <v>34400</v>
+      </c>
+      <c r="I111">
+        <v>7000</v>
+      </c>
+      <c r="J111">
+        <v>1000</v>
+      </c>
+      <c r="R111">
+        <v>5000</v>
+      </c>
+      <c r="V111">
+        <v>1000</v>
+      </c>
+      <c r="W111">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:23">
+      <c r="A112" s="2">
+        <v>45147</v>
+      </c>
+      <c r="D112">
+        <v>168500</v>
+      </c>
+      <c r="F112">
+        <v>20500</v>
+      </c>
+      <c r="I112">
+        <v>7000</v>
+      </c>
+      <c r="J112">
+        <v>1000</v>
+      </c>
+      <c r="K112">
+        <v>80000</v>
+      </c>
+      <c r="R112">
+        <v>28000</v>
+      </c>
+      <c r="U112">
+        <v>16000</v>
+      </c>
+      <c r="V112">
+        <v>397000</v>
+      </c>
+      <c r="W112">
+        <v>46500</v>
+      </c>
+    </row>
+    <row r="113" spans="1:23">
+      <c r="A113" s="2">
+        <v>45148</v>
+      </c>
+      <c r="C113">
+        <v>92000</v>
+      </c>
+      <c r="D113">
+        <v>71450</v>
+      </c>
+      <c r="F113">
+        <v>272000</v>
+      </c>
+      <c r="J113">
+        <v>1000</v>
+      </c>
+      <c r="K113">
+        <v>40000</v>
+      </c>
+      <c r="M113">
+        <v>300000</v>
+      </c>
+      <c r="O113">
+        <v>25000</v>
+      </c>
+      <c r="R113">
+        <v>42000</v>
+      </c>
+      <c r="U113">
+        <v>130000</v>
+      </c>
+      <c r="V113">
+        <v>80000</v>
+      </c>
+      <c r="W113">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:23">
+      <c r="A114" s="2">
+        <v>45149</v>
+      </c>
+      <c r="D114">
+        <v>69600</v>
+      </c>
+      <c r="F114">
+        <v>417500</v>
+      </c>
+      <c r="I114">
+        <v>10500</v>
+      </c>
+      <c r="J114">
+        <v>1000</v>
+      </c>
+      <c r="R114">
+        <v>6500</v>
+      </c>
+      <c r="T114">
+        <v>1500</v>
+      </c>
+      <c r="U114">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:23">
+      <c r="A115" s="2">
+        <v>45150</v>
+      </c>
+      <c r="D115">
+        <v>122500</v>
+      </c>
+      <c r="F115">
+        <v>92600</v>
+      </c>
+      <c r="I115">
+        <v>3500</v>
+      </c>
+      <c r="J115">
+        <v>1000</v>
+      </c>
+      <c r="R115">
+        <v>14500</v>
+      </c>
+      <c r="U115">
+        <v>39000</v>
+      </c>
+      <c r="V115">
+        <v>135000</v>
+      </c>
+      <c r="W115">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:23">
+      <c r="A116" s="2">
+        <v>45151</v>
+      </c>
+      <c r="C116">
+        <v>92000</v>
+      </c>
+      <c r="D116">
+        <v>159375</v>
+      </c>
+      <c r="F116">
+        <v>529400</v>
+      </c>
+      <c r="G116">
+        <v>1726500</v>
+      </c>
+      <c r="I116">
+        <v>9000</v>
+      </c>
+      <c r="J116">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:23">
+      <c r="A117" s="2">
+        <v>45152</v>
+      </c>
+      <c r="D117">
+        <v>140175</v>
+      </c>
+      <c r="F117">
+        <v>49100</v>
+      </c>
+      <c r="J117">
+        <v>1000</v>
+      </c>
+      <c r="N117">
+        <v>1000</v>
+      </c>
+      <c r="R117">
+        <v>4500</v>
+      </c>
+      <c r="V117">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:23">
+      <c r="A118" s="2">
+        <v>45153</v>
+      </c>
+      <c r="D118">
+        <v>16500</v>
+      </c>
+      <c r="F118">
+        <v>4800</v>
+      </c>
+      <c r="I118">
+        <v>10500</v>
+      </c>
+      <c r="J118">
+        <v>1000</v>
+      </c>
+      <c r="R118">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="119" spans="1:23">
+      <c r="A119" s="2">
+        <v>45154</v>
+      </c>
+      <c r="D119">
+        <v>110250</v>
+      </c>
+      <c r="F119">
+        <v>961400</v>
+      </c>
+      <c r="I119">
+        <v>10500</v>
+      </c>
+      <c r="J119">
+        <v>1000</v>
+      </c>
+      <c r="O119">
+        <v>55000</v>
+      </c>
+      <c r="R119">
+        <v>56000</v>
+      </c>
+      <c r="S119">
+        <v>10000</v>
+      </c>
+      <c r="U119">
+        <v>40000</v>
+      </c>
+      <c r="V119">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:23">
+      <c r="A120" s="2">
+        <v>45155</v>
+      </c>
+      <c r="C120">
+        <v>92000</v>
+      </c>
+      <c r="D120">
+        <v>155600</v>
+      </c>
+      <c r="F120">
+        <v>33900</v>
+      </c>
+      <c r="I120">
+        <v>10500</v>
+      </c>
+      <c r="J120">
+        <v>1000</v>
+      </c>
+      <c r="K120">
+        <v>30000</v>
+      </c>
+      <c r="Q120">
+        <v>2000</v>
+      </c>
+      <c r="R120">
+        <v>9000</v>
+      </c>
+      <c r="T120">
+        <v>1500</v>
+      </c>
+      <c r="V120">
+        <v>338800</v>
+      </c>
+      <c r="W120">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:23">
+      <c r="A121" s="2">
+        <v>45156</v>
+      </c>
+      <c r="D121">
+        <v>128700</v>
+      </c>
+      <c r="I121">
+        <v>10500</v>
+      </c>
+      <c r="J121">
+        <v>1000</v>
+      </c>
+      <c r="R121">
+        <v>28500</v>
+      </c>
+      <c r="S121">
+        <v>1000</v>
+      </c>
+      <c r="U121">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:23">
+      <c r="A122" s="2">
+        <v>45157</v>
+      </c>
+      <c r="D122">
+        <v>100550</v>
+      </c>
+      <c r="I122">
+        <v>7000</v>
+      </c>
+      <c r="J122">
+        <v>1000</v>
+      </c>
+      <c r="R122">
+        <v>3000</v>
+      </c>
+      <c r="T122">
+        <v>1500</v>
+      </c>
+      <c r="W122">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23">
+      <c r="A123" s="2">
+        <v>45158</v>
+      </c>
+      <c r="C123">
+        <v>77500</v>
+      </c>
+      <c r="D123">
+        <v>102225</v>
+      </c>
+      <c r="G123">
+        <v>2060800</v>
+      </c>
+      <c r="I123">
+        <v>10500</v>
+      </c>
+      <c r="T123">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23">
+      <c r="A124" s="2">
+        <v>45159</v>
+      </c>
+      <c r="D124">
+        <v>97750</v>
+      </c>
+      <c r="E124">
+        <v>37250</v>
+      </c>
+      <c r="J124">
+        <v>1000</v>
+      </c>
+      <c r="R124">
+        <v>9000</v>
+      </c>
+      <c r="V124">
+        <v>765000</v>
+      </c>
+      <c r="W124">
+        <v>185000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23">
+      <c r="A125" s="2">
+        <v>45160</v>
+      </c>
+      <c r="D125">
+        <v>13000</v>
+      </c>
+      <c r="F125">
+        <v>240900</v>
+      </c>
+      <c r="I125">
+        <v>10500</v>
+      </c>
+      <c r="J125">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23">
+      <c r="A126" s="2">
+        <v>45161</v>
+      </c>
+      <c r="C126">
+        <v>77500</v>
+      </c>
+      <c r="D126">
+        <v>132150</v>
+      </c>
+      <c r="F126">
+        <v>518700</v>
+      </c>
+      <c r="I126">
+        <v>10500</v>
+      </c>
+      <c r="J126">
+        <v>1000</v>
+      </c>
+      <c r="K126">
+        <v>160000</v>
+      </c>
+      <c r="Q126">
+        <v>3000</v>
+      </c>
+      <c r="R126">
+        <v>30500</v>
+      </c>
+      <c r="T126">
+        <v>2100</v>
+      </c>
+      <c r="U126">
+        <v>145650</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23">
+      <c r="A127" s="2">
+        <v>45162</v>
+      </c>
+      <c r="D127">
+        <v>119400</v>
+      </c>
+      <c r="F127">
+        <v>105600</v>
+      </c>
+      <c r="J127">
+        <v>1000</v>
+      </c>
+      <c r="K127">
+        <v>30000</v>
+      </c>
+      <c r="R127">
+        <v>9000</v>
+      </c>
+      <c r="V127">
+        <v>51750</v>
+      </c>
+      <c r="W127">
+        <v>57500</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23">
+      <c r="A128" s="2">
+        <v>45163</v>
+      </c>
+      <c r="D128">
+        <v>96900</v>
+      </c>
+      <c r="F128">
+        <v>86000</v>
+      </c>
+      <c r="I128">
+        <v>21000</v>
+      </c>
+      <c r="W128">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23">
+      <c r="A129" s="2">
+        <v>45164</v>
+      </c>
+      <c r="C129">
+        <v>77500</v>
+      </c>
+      <c r="D129">
+        <v>118225</v>
+      </c>
+      <c r="F129">
+        <v>545300</v>
+      </c>
+      <c r="I129">
+        <v>6500</v>
+      </c>
+      <c r="J129">
+        <v>1000</v>
+      </c>
+      <c r="R129">
+        <v>5500</v>
+      </c>
+      <c r="W129">
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23">
+      <c r="A130" s="2">
+        <v>45165</v>
+      </c>
+      <c r="D130">
+        <v>95650</v>
+      </c>
+      <c r="F130">
+        <v>103000</v>
+      </c>
+      <c r="G130">
+        <v>1643150</v>
+      </c>
+      <c r="I130">
+        <v>10500</v>
+      </c>
+      <c r="J130">
+        <v>1000</v>
+      </c>
+      <c r="M130">
+        <v>30000</v>
+      </c>
+      <c r="R130">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:23">
+      <c r="A131" s="2">
+        <v>45166</v>
+      </c>
+      <c r="C131">
+        <v>77500</v>
+      </c>
+      <c r="D131">
+        <v>223500</v>
+      </c>
+      <c r="F131">
+        <v>2500</v>
+      </c>
+      <c r="I131">
+        <v>2000</v>
+      </c>
+      <c r="J131">
+        <v>500</v>
+      </c>
+      <c r="M131">
+        <v>300000</v>
+      </c>
+      <c r="R131">
+        <v>500</v>
+      </c>
+      <c r="S131">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23">
+      <c r="A132" s="2">
+        <v>45167</v>
+      </c>
+      <c r="D132">
+        <v>35000</v>
+      </c>
+      <c r="F132">
+        <v>29000</v>
+      </c>
+      <c r="I132">
+        <v>10500</v>
+      </c>
+      <c r="O132">
+        <v>5000</v>
+      </c>
+      <c r="R132">
+        <v>9000</v>
+      </c>
+      <c r="V132">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23">
+      <c r="A133" s="2">
+        <v>45168</v>
+      </c>
+      <c r="D133">
+        <v>101550</v>
+      </c>
+      <c r="F133">
+        <v>1395200</v>
+      </c>
+      <c r="I133">
+        <v>10500</v>
+      </c>
+      <c r="J133">
+        <v>1000</v>
+      </c>
+      <c r="K133">
+        <v>60000</v>
+      </c>
+      <c r="R133">
+        <v>105500</v>
+      </c>
+      <c r="S133">
+        <v>3000</v>
+      </c>
+      <c r="V133">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23">
+      <c r="A134" s="2">
+        <v>45169</v>
+      </c>
+      <c r="C134">
+        <v>77500</v>
+      </c>
+      <c r="D134">
+        <v>69950</v>
+      </c>
+      <c r="F134">
+        <v>42500</v>
+      </c>
+      <c r="J134">
+        <v>1000</v>
+      </c>
+      <c r="K134">
+        <v>30000</v>
+      </c>
+      <c r="P134">
+        <v>200000</v>
+      </c>
+      <c r="R134">
+        <v>6500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update du mois d'octobre
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -444,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W164"/>
+  <dimension ref="A1:W195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4660,6 +4660,785 @@
         <v>200000</v>
       </c>
     </row>
+    <row r="165" spans="1:23">
+      <c r="A165" s="2">
+        <v>45200</v>
+      </c>
+      <c r="D165">
+        <v>65850</v>
+      </c>
+      <c r="F165">
+        <v>123500</v>
+      </c>
+      <c r="G165">
+        <v>2027450</v>
+      </c>
+      <c r="I165">
+        <v>14000</v>
+      </c>
+      <c r="J165">
+        <v>1000</v>
+      </c>
+      <c r="R165">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23">
+      <c r="A166" s="2">
+        <v>45201</v>
+      </c>
+      <c r="C166">
+        <v>77500</v>
+      </c>
+      <c r="D166">
+        <v>215525</v>
+      </c>
+      <c r="J166">
+        <v>1000</v>
+      </c>
+      <c r="R166">
+        <v>9000</v>
+      </c>
+      <c r="S166">
+        <v>4400</v>
+      </c>
+      <c r="W166">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23">
+      <c r="A167" s="2">
+        <v>45202</v>
+      </c>
+      <c r="D167">
+        <v>19000</v>
+      </c>
+      <c r="F167">
+        <v>209000</v>
+      </c>
+      <c r="I167">
+        <v>10500</v>
+      </c>
+      <c r="J167">
+        <v>1000</v>
+      </c>
+      <c r="V167">
+        <v>247500</v>
+      </c>
+    </row>
+    <row r="168" spans="1:23">
+      <c r="A168" s="2">
+        <v>45203</v>
+      </c>
+      <c r="D168">
+        <v>79350</v>
+      </c>
+      <c r="I168">
+        <v>7000</v>
+      </c>
+      <c r="J168">
+        <v>1000</v>
+      </c>
+      <c r="K168">
+        <v>50000</v>
+      </c>
+      <c r="M168">
+        <v>250000</v>
+      </c>
+      <c r="Q168">
+        <v>1500</v>
+      </c>
+      <c r="R168">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="169" spans="1:23">
+      <c r="A169" s="2">
+        <v>45204</v>
+      </c>
+      <c r="C169">
+        <v>77500</v>
+      </c>
+      <c r="D169">
+        <v>121550</v>
+      </c>
+      <c r="F169">
+        <v>886000</v>
+      </c>
+      <c r="I169">
+        <v>5000</v>
+      </c>
+      <c r="J169">
+        <v>1000</v>
+      </c>
+      <c r="K169">
+        <v>55000</v>
+      </c>
+      <c r="V169">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="170" spans="1:23">
+      <c r="A170" s="2">
+        <v>45205</v>
+      </c>
+      <c r="D170">
+        <v>99750</v>
+      </c>
+      <c r="F170">
+        <v>187000</v>
+      </c>
+      <c r="I170">
+        <v>10500</v>
+      </c>
+      <c r="J170">
+        <v>1000</v>
+      </c>
+      <c r="R170">
+        <v>42000</v>
+      </c>
+      <c r="U170">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="171" spans="1:23">
+      <c r="A171" s="2">
+        <v>45206</v>
+      </c>
+      <c r="D171">
+        <v>112100</v>
+      </c>
+      <c r="F171">
+        <v>118400</v>
+      </c>
+      <c r="I171">
+        <v>8750</v>
+      </c>
+      <c r="J171">
+        <v>1000</v>
+      </c>
+      <c r="R171">
+        <v>30000</v>
+      </c>
+      <c r="S171">
+        <v>600</v>
+      </c>
+      <c r="V171">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="172" spans="1:23">
+      <c r="A172" s="2">
+        <v>45207</v>
+      </c>
+      <c r="C172">
+        <v>77500</v>
+      </c>
+      <c r="D172">
+        <v>54450</v>
+      </c>
+      <c r="F172">
+        <v>295500</v>
+      </c>
+      <c r="G172">
+        <v>1856550</v>
+      </c>
+      <c r="I172">
+        <v>17500</v>
+      </c>
+      <c r="J172">
+        <v>1000</v>
+      </c>
+      <c r="S172">
+        <v>160000</v>
+      </c>
+      <c r="T172">
+        <v>500</v>
+      </c>
+      <c r="V172">
+        <v>435000</v>
+      </c>
+    </row>
+    <row r="173" spans="1:23">
+      <c r="A173" s="2">
+        <v>45208</v>
+      </c>
+      <c r="C173">
+        <v>15000</v>
+      </c>
+      <c r="D173">
+        <v>106950</v>
+      </c>
+      <c r="E173">
+        <v>37250</v>
+      </c>
+      <c r="F173">
+        <v>30000</v>
+      </c>
+      <c r="J173">
+        <v>1000</v>
+      </c>
+      <c r="R173">
+        <v>10600</v>
+      </c>
+      <c r="U173">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23">
+      <c r="A174" s="2">
+        <v>45209</v>
+      </c>
+      <c r="D174">
+        <v>17500</v>
+      </c>
+      <c r="F174">
+        <v>41000</v>
+      </c>
+      <c r="I174">
+        <v>10500</v>
+      </c>
+      <c r="J174">
+        <v>1000</v>
+      </c>
+      <c r="R174">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23">
+      <c r="A175" s="2">
+        <v>45210</v>
+      </c>
+      <c r="C175">
+        <v>77500</v>
+      </c>
+      <c r="D175">
+        <v>58125</v>
+      </c>
+      <c r="F175">
+        <v>620500</v>
+      </c>
+      <c r="I175">
+        <v>10500</v>
+      </c>
+      <c r="J175">
+        <v>1000</v>
+      </c>
+      <c r="K175">
+        <v>90000</v>
+      </c>
+      <c r="R175">
+        <v>10600</v>
+      </c>
+      <c r="U175">
+        <v>90000</v>
+      </c>
+      <c r="V175">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="176" spans="1:23">
+      <c r="A176" s="2">
+        <v>45211</v>
+      </c>
+      <c r="D176">
+        <v>163700</v>
+      </c>
+      <c r="F176">
+        <v>126400</v>
+      </c>
+      <c r="I176">
+        <v>10500</v>
+      </c>
+      <c r="J176">
+        <v>1000</v>
+      </c>
+      <c r="K176">
+        <v>35000</v>
+      </c>
+      <c r="Q176">
+        <v>1400</v>
+      </c>
+      <c r="R176">
+        <v>10600</v>
+      </c>
+    </row>
+    <row r="177" spans="1:23">
+      <c r="A177" s="2">
+        <v>45212</v>
+      </c>
+      <c r="D177">
+        <v>149650</v>
+      </c>
+      <c r="F177">
+        <v>393200</v>
+      </c>
+      <c r="J177">
+        <v>1000</v>
+      </c>
+      <c r="T177">
+        <v>2000</v>
+      </c>
+      <c r="U177">
+        <v>157800</v>
+      </c>
+    </row>
+    <row r="178" spans="1:23">
+      <c r="A178" s="2">
+        <v>45213</v>
+      </c>
+      <c r="C178">
+        <v>77500</v>
+      </c>
+      <c r="D178">
+        <v>82600</v>
+      </c>
+      <c r="F178">
+        <v>82000</v>
+      </c>
+      <c r="J178">
+        <v>1000</v>
+      </c>
+      <c r="M178">
+        <v>250000</v>
+      </c>
+      <c r="R178">
+        <v>9000</v>
+      </c>
+      <c r="U178">
+        <v>80700</v>
+      </c>
+      <c r="V178">
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="179" spans="1:23">
+      <c r="A179" s="2">
+        <v>45214</v>
+      </c>
+      <c r="C179">
+        <v>77500</v>
+      </c>
+      <c r="D179">
+        <v>155100</v>
+      </c>
+      <c r="F179">
+        <v>134000</v>
+      </c>
+      <c r="G179">
+        <v>1440000</v>
+      </c>
+      <c r="I179">
+        <v>31500</v>
+      </c>
+      <c r="J179">
+        <v>1000</v>
+      </c>
+      <c r="R179">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="180" spans="1:23">
+      <c r="A180" s="2">
+        <v>45215</v>
+      </c>
+      <c r="D180">
+        <v>141650</v>
+      </c>
+      <c r="J180">
+        <v>1000</v>
+      </c>
+      <c r="O180">
+        <v>55000</v>
+      </c>
+      <c r="R180">
+        <v>39500</v>
+      </c>
+      <c r="T180">
+        <v>5000</v>
+      </c>
+      <c r="W180">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="181" spans="1:23">
+      <c r="A181" s="2">
+        <v>45216</v>
+      </c>
+      <c r="D181">
+        <v>19000</v>
+      </c>
+      <c r="F181">
+        <v>336000</v>
+      </c>
+      <c r="J181">
+        <v>1000</v>
+      </c>
+      <c r="Q181">
+        <v>2000</v>
+      </c>
+      <c r="R181">
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="182" spans="1:23">
+      <c r="A182" s="2">
+        <v>45217</v>
+      </c>
+      <c r="D182">
+        <v>100050</v>
+      </c>
+      <c r="F182">
+        <v>65400</v>
+      </c>
+      <c r="I182">
+        <v>10000</v>
+      </c>
+      <c r="J182">
+        <v>1000</v>
+      </c>
+      <c r="K182">
+        <v>50000</v>
+      </c>
+      <c r="Q182">
+        <v>1000</v>
+      </c>
+      <c r="R182">
+        <v>4100</v>
+      </c>
+      <c r="T182">
+        <v>1000</v>
+      </c>
+      <c r="V182">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="183" spans="1:23">
+      <c r="A183" s="2">
+        <v>45218</v>
+      </c>
+      <c r="C183">
+        <v>77500</v>
+      </c>
+      <c r="D183">
+        <v>170400</v>
+      </c>
+      <c r="F183">
+        <v>73500</v>
+      </c>
+      <c r="J183">
+        <v>1000</v>
+      </c>
+      <c r="K183">
+        <v>35000</v>
+      </c>
+      <c r="R183">
+        <v>9000</v>
+      </c>
+      <c r="V183">
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="184" spans="1:23">
+      <c r="A184" s="2">
+        <v>45219</v>
+      </c>
+      <c r="D184">
+        <v>68350</v>
+      </c>
+      <c r="F184">
+        <v>413000</v>
+      </c>
+      <c r="I184">
+        <v>10500</v>
+      </c>
+      <c r="J184">
+        <v>1000</v>
+      </c>
+      <c r="R184">
+        <v>10600</v>
+      </c>
+      <c r="V184">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="185" spans="1:23">
+      <c r="A185" s="2">
+        <v>45220</v>
+      </c>
+      <c r="C185">
+        <v>77500</v>
+      </c>
+      <c r="D185">
+        <v>145650</v>
+      </c>
+      <c r="I185">
+        <v>10500</v>
+      </c>
+      <c r="J185">
+        <v>1000</v>
+      </c>
+      <c r="M185">
+        <v>75000</v>
+      </c>
+      <c r="V185">
+        <v>62000</v>
+      </c>
+    </row>
+    <row r="186" spans="1:23">
+      <c r="A186" s="2">
+        <v>45221</v>
+      </c>
+      <c r="D186">
+        <v>115250</v>
+      </c>
+      <c r="F186">
+        <v>57000</v>
+      </c>
+      <c r="G186">
+        <v>1696900</v>
+      </c>
+      <c r="I186">
+        <v>17500</v>
+      </c>
+      <c r="J186">
+        <v>1000</v>
+      </c>
+      <c r="R186">
+        <v>2800</v>
+      </c>
+      <c r="V186">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:23">
+      <c r="A187" s="2">
+        <v>45222</v>
+      </c>
+      <c r="D187">
+        <v>203050</v>
+      </c>
+      <c r="F187">
+        <v>642500</v>
+      </c>
+      <c r="J187">
+        <v>1000</v>
+      </c>
+      <c r="R187">
+        <v>64000</v>
+      </c>
+      <c r="S187">
+        <v>9000</v>
+      </c>
+      <c r="U187">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="188" spans="1:23">
+      <c r="A188" s="2">
+        <v>45223</v>
+      </c>
+      <c r="D188">
+        <v>25500</v>
+      </c>
+      <c r="F188">
+        <v>89000</v>
+      </c>
+      <c r="I188">
+        <v>10500</v>
+      </c>
+      <c r="J188">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="189" spans="1:23">
+      <c r="A189" s="2">
+        <v>45224</v>
+      </c>
+      <c r="C189">
+        <v>77500</v>
+      </c>
+      <c r="D189">
+        <v>120325</v>
+      </c>
+      <c r="F189">
+        <v>51500</v>
+      </c>
+      <c r="I189">
+        <v>10500</v>
+      </c>
+      <c r="J189">
+        <v>1000</v>
+      </c>
+      <c r="K189">
+        <v>60000</v>
+      </c>
+      <c r="R189">
+        <v>9000</v>
+      </c>
+      <c r="S189">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="190" spans="1:23">
+      <c r="A190" s="2">
+        <v>45225</v>
+      </c>
+      <c r="D190">
+        <v>121800</v>
+      </c>
+      <c r="F190">
+        <v>858900</v>
+      </c>
+      <c r="I190">
+        <v>10500</v>
+      </c>
+      <c r="J190">
+        <v>2000</v>
+      </c>
+      <c r="K190">
+        <v>35000</v>
+      </c>
+      <c r="R190">
+        <v>10600</v>
+      </c>
+      <c r="T190">
+        <v>11000</v>
+      </c>
+      <c r="U190">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="191" spans="1:23">
+      <c r="A191" s="2">
+        <v>45226</v>
+      </c>
+      <c r="D191">
+        <v>64475</v>
+      </c>
+      <c r="E191">
+        <v>37250</v>
+      </c>
+      <c r="F191">
+        <v>38000</v>
+      </c>
+      <c r="I191">
+        <v>10500</v>
+      </c>
+      <c r="J191">
+        <v>1000</v>
+      </c>
+      <c r="M191">
+        <v>300000</v>
+      </c>
+      <c r="R191">
+        <v>14000</v>
+      </c>
+      <c r="T191">
+        <v>1000</v>
+      </c>
+      <c r="V191">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="192" spans="1:23">
+      <c r="A192" s="2">
+        <v>45227</v>
+      </c>
+      <c r="C192">
+        <v>77500</v>
+      </c>
+      <c r="D192">
+        <v>180700</v>
+      </c>
+      <c r="F192">
+        <v>31100</v>
+      </c>
+      <c r="I192">
+        <v>7000</v>
+      </c>
+      <c r="J192">
+        <v>1000</v>
+      </c>
+      <c r="R192">
+        <v>30000</v>
+      </c>
+      <c r="T192">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="193" spans="1:23">
+      <c r="A193" s="2">
+        <v>45228</v>
+      </c>
+      <c r="D193">
+        <v>102700</v>
+      </c>
+      <c r="F193">
+        <v>57000</v>
+      </c>
+      <c r="G193">
+        <v>919250</v>
+      </c>
+      <c r="I193">
+        <v>17500</v>
+      </c>
+      <c r="J193">
+        <v>1000</v>
+      </c>
+      <c r="R193">
+        <v>9000</v>
+      </c>
+      <c r="T193">
+        <v>5000</v>
+      </c>
+      <c r="W193">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:23">
+      <c r="A194" s="2">
+        <v>45229</v>
+      </c>
+      <c r="D194">
+        <v>62800</v>
+      </c>
+      <c r="F194">
+        <v>47500</v>
+      </c>
+      <c r="J194">
+        <v>1000</v>
+      </c>
+      <c r="W194">
+        <v>289500</v>
+      </c>
+    </row>
+    <row r="195" spans="1:23">
+      <c r="A195" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C195">
+        <v>77.5</v>
+      </c>
+      <c r="D195">
+        <v>25.5</v>
+      </c>
+      <c r="F195">
+        <v>7</v>
+      </c>
+      <c r="J195">
+        <v>1000</v>
+      </c>
+      <c r="P195">
+        <v>200000</v>
+      </c>
+      <c r="U195">
+        <v>42000</v>
+      </c>
+      <c r="V195">
+        <v>10000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update du 13 novembre 2023
</commit_message>
<xml_diff>
--- a/Analyse.xlsx
+++ b/Analyse.xlsx
@@ -746,9 +746,6 @@
       <c r="D12">
         <v>111150</v>
       </c>
-      <c r="F12">
-        <v>470250</v>
-      </c>
       <c r="T12">
         <v>3000</v>
       </c>
@@ -5418,13 +5415,13 @@
         <v>45230</v>
       </c>
       <c r="C195">
-        <v>77.5</v>
+        <v>77500</v>
       </c>
       <c r="D195">
-        <v>25.5</v>
+        <v>25500</v>
       </c>
       <c r="F195">
-        <v>7</v>
+        <v>7000</v>
       </c>
       <c r="J195">
         <v>1000</v>

</xml_diff>